<commit_message>
adding team backlog + testcases sheet
</commit_message>
<xml_diff>
--- a/Documents/TeamBacklog_TestCases.xlsx
+++ b/Documents/TeamBacklog_TestCases.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elwady\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elwady\Downloads\SimpleATMMachine-Project-Atmega32-Sprints\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AA70320-6320-49B2-B50E-332C40AA5845}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F0556DD-E249-4432-AA7A-36507CBCE184}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1248" yWindow="2676" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team Backlog" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="50">
   <si>
     <t>Task Name</t>
   </si>
@@ -73,60 +73,9 @@
     <t>Actual Results</t>
   </si>
   <si>
-    <t xml:space="preserve">Testing Timer delay + timer interrupt </t>
-  </si>
-  <si>
-    <t>led 0 toggle after 1 sec using TIMER_delay then led 1 toggle every 2 sec using ovf interrupt</t>
-  </si>
-  <si>
-    <t>Same as expected</t>
-  </si>
-  <si>
     <t>PASS</t>
   </si>
   <si>
-    <t xml:space="preserve">Testing LM35 </t>
-  </si>
-  <si>
-    <t>when temp &gt; 25 led 1 on led 2 off, when temp &lt;= 25 led 1 off led 2 on.</t>
-  </si>
-  <si>
-    <t>Testing Keypad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">representing keypad's buttons value binary on 4 leds  </t>
-  </si>
-  <si>
-    <t>Testing Application; press set button, wait 2 seconds, press reset button, wait two seconds press adjust, wait 10 secs,  press increment button.</t>
-  </si>
-  <si>
-    <t>after pressing set button, buzzer will be on + bell shape at the beginning, after pressing reset button and waiting 10 seconds it will timeout from setting state and go to idle state of showing current temp + bell shape if it's higher than desired temp, after pressing increment button will print  this operation is not allowed.</t>
-  </si>
-  <si>
-    <t>Testing Application; During setting state press increment till it exceeds 35</t>
-  </si>
-  <si>
-    <t xml:space="preserve">with every press a bell shape will be deleted from the second line representing number of degrees after reaching 18 decrement button will not have any effect  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">with every press a bell shape will be drawn in the second line representing number of degrees after reaching 35 increment button will not have any effect  </t>
-  </si>
-  <si>
-    <t>Testing Application; During setting state press decrement till it exceeds 18</t>
-  </si>
-  <si>
-    <t>Testing Application; During Idle state increase and decrease exposed temperature to temperature sensor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LCD will print current temperature as the temperature measured from temperature sensor </t>
-  </si>
-  <si>
-    <t>It sometimes prints the same temperature and sometimes prints a higher or lower temperature by 1 degree</t>
-  </si>
-  <si>
-    <t>NEUTRAL</t>
-  </si>
-  <si>
     <t>UART Design</t>
   </si>
   <si>
@@ -161,13 +110,79 @@
   </si>
   <si>
     <t>ATM Application Development</t>
+  </si>
+  <si>
+    <t>Pressing all inputs before getting the trigger signal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entering wrong pin three times </t>
+  </si>
+  <si>
+    <t>CARD</t>
+  </si>
+  <si>
+    <t>Entering invalid PIN length</t>
+  </si>
+  <si>
+    <t>Entering correct pin</t>
+  </si>
+  <si>
+    <t>ATM</t>
+  </si>
+  <si>
+    <t>Enter PAN &gt; 19 numeric characters</t>
+  </si>
+  <si>
+    <t>Enter PAN &lt; 16 numeric characters</t>
+  </si>
+  <si>
+    <t>Enter PAN with alphabetic characters</t>
+  </si>
+  <si>
+    <t>Enter Correct PAN</t>
+  </si>
+  <si>
+    <t>Enter PIN &gt; 4 numeric digits</t>
+  </si>
+  <si>
+    <t>Enter PIN &lt; 4 numeric digits</t>
+  </si>
+  <si>
+    <t>Enter PIN alphabetic digits</t>
+  </si>
+  <si>
+    <t>Enter different PINs in confirmation</t>
+  </si>
+  <si>
+    <t>Enter Correct PIN</t>
+  </si>
+  <si>
+    <t>Enter correct PIN confirmation</t>
+  </si>
+  <si>
+    <t>Application</t>
+  </si>
+  <si>
+    <t>Approved User Story Mention balance before the transaction</t>
+  </si>
+  <si>
+    <t>Fraud Card</t>
+  </si>
+  <si>
+    <t>Stolen Card</t>
+  </si>
+  <si>
+    <t>Max limit exceeded</t>
+  </si>
+  <si>
+    <t>Insufficient fund</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -190,20 +205,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -213,11 +221,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
     <fill>
@@ -297,15 +300,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -321,13 +323,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -338,39 +334,38 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="4">
-    <cellStyle name="60% - Accent1" xfId="3" builtinId="32"/>
+  <cellStyles count="3">
+    <cellStyle name="60% - Accent1" xfId="2" builtinId="32"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="11">
@@ -435,8 +430,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table5" displayName="Table5" ref="A1:E8" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:E8" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table5" displayName="Table5" ref="A1:E23" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:E23" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Test Case ID" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Description / steps" dataDxfId="3"/>
@@ -747,7 +742,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9:E9"/>
     </sheetView>
   </sheetViews>
@@ -779,7 +774,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -787,16 +782,16 @@
       <c r="C2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="12">
+      <c r="D2" s="10">
         <v>45051</v>
       </c>
-      <c r="E2" s="12">
+      <c r="E2" s="10">
         <v>45082</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -804,16 +799,16 @@
       <c r="C3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="12">
+      <c r="D3" s="10">
         <v>45051</v>
       </c>
-      <c r="E3" s="12">
+      <c r="E3" s="10">
         <v>45082</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -821,16 +816,16 @@
       <c r="C4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="10">
         <v>45051</v>
       </c>
-      <c r="E4" s="12">
+      <c r="E4" s="10">
         <v>45082</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -838,16 +833,16 @@
       <c r="C5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="10">
         <v>45051</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="10">
         <v>45082</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
@@ -855,16 +850,16 @@
       <c r="C6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6" s="10">
         <v>45051</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E6" s="10">
         <v>45082</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
@@ -872,16 +867,16 @@
       <c r="C7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="10">
         <v>45051</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="10">
         <v>45082</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
@@ -889,16 +884,16 @@
       <c r="C8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="12">
+      <c r="D8" s="10">
         <v>45051</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8" s="10">
         <v>45082</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
         <v>5</v>
@@ -906,110 +901,110 @@
       <c r="C9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="12">
+      <c r="D9" s="10">
         <v>45051</v>
       </c>
-      <c r="E9" s="12">
+      <c r="E9" s="10">
         <v>45082</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="B10" s="21" t="s">
+      <c r="A10" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="22">
+      <c r="D10" s="20">
         <v>45051</v>
       </c>
-      <c r="E10" s="18">
+      <c r="E10" s="16">
         <v>45082</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="B11" s="9" t="s">
+      <c r="A11" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="13">
+      <c r="D11" s="11">
         <v>45051</v>
       </c>
-      <c r="E11" s="20">
+      <c r="E11" s="18">
         <v>45082</v>
       </c>
     </row>
     <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="16"/>
-      <c r="B12" s="16"/>
+      <c r="A12" s="14"/>
+      <c r="B12" s="14"/>
       <c r="C12" s="3"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="13"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="B13" s="21" t="s">
+      <c r="A13" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="22">
+      <c r="D13" s="20">
         <v>45051</v>
       </c>
-      <c r="E13" s="18">
+      <c r="E13" s="16">
         <v>45082</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="B14" s="9" t="s">
+      <c r="A14" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="24">
+      <c r="D14" s="22">
         <v>45051</v>
       </c>
-      <c r="E14" s="14">
+      <c r="E14" s="12">
         <v>45082</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="23" t="s">
+      <c r="A15" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="21" t="s">
+      <c r="B15" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="22">
+      <c r="D15" s="20">
         <v>45051</v>
       </c>
-      <c r="E15" s="18">
+      <c r="E15" s="16">
         <v>45082</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E16" s="19"/>
+      <c r="E16" s="17"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
@@ -1020,18 +1015,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.88671875" customWidth="1"/>
-    <col min="2" max="2" width="37.5546875" customWidth="1"/>
+    <col min="2" max="2" width="47" customWidth="1"/>
     <col min="3" max="3" width="49.44140625" customWidth="1"/>
-    <col min="4" max="4" width="22" customWidth="1"/>
+    <col min="4" max="4" width="40.33203125" customWidth="1"/>
     <col min="5" max="5" width="9.77734375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1052,123 +1047,278 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="5">
+      <c r="B3" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="5">
         <v>2</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="6">
+      <c r="B4" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="6">
         <v>3</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A5" s="6">
+      <c r="B5" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="6">
         <v>4</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="5">
+      <c r="B6" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="5">
+        <v>1</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="5">
+        <v>2</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="5">
+        <v>3</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="5">
+        <v>4</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="5">
         <v>5</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="5">
+      <c r="B12" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="5">
         <v>6</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="72" x14ac:dyDescent="0.3">
-      <c r="A8" s="5">
+      <c r="B13" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="5">
         <v>7</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>32</v>
+      <c r="B14" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="5">
+        <v>8</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="5">
+        <v>9</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="5">
+        <v>10</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="3"/>
+    </row>
+    <row r="19" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="5">
+        <v>1</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="5">
+        <v>2</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="5">
+        <v>3</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="5">
+        <v>4</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="5">
+        <v>5</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>